<commit_message>
Added support to differentiation by gender
</commit_message>
<xml_diff>
--- a/Q145_diagrams.xlsx
+++ b/Q145_diagrams.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="20">
   <si>
     <t>response</t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>WeFarm</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Men</t>
+  </si>
+  <si>
+    <t>Women</t>
   </si>
 </sst>
 </file>
@@ -247,7 +256,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Q145'!$C$1</c:f>
+              <c:f>'Q145'!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -268,7 +277,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Q145'!$B$2:$B$15</c:f>
+              <c:f>'Q145'!$B$3:$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -318,7 +327,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Q145'!$C$2:$C$15</c:f>
+              <c:f>'Q145'!$C$3:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -373,7 +382,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Q145'!$D$1</c:f>
+              <c:f>'Q145'!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -394,7 +403,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Q145'!$B$2:$B$15</c:f>
+              <c:f>'Q145'!$B$3:$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -444,7 +453,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Q145'!$D$2:$D$15</c:f>
+              <c:f>'Q145'!$D$3:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -504,11 +513,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2106493552"/>
-        <c:axId val="-2101457712"/>
+        <c:axId val="-2063787312"/>
+        <c:axId val="-2063625344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2106493552"/>
+        <c:axId val="-2063787312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -551,7 +560,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2101457712"/>
+        <c:crossAx val="-2063625344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -559,7 +568,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2101457712"/>
+        <c:axId val="-2063625344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -610,7 +619,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2106493552"/>
+        <c:crossAx val="-2063787312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1239,15 +1248,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>17182</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1532,219 +1541,648 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>0.14754098360655701</v>
-      </c>
-      <c r="D2">
-        <v>9.7560975609756097E-3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>4.59016393442623E-2</v>
+        <v>0.14754098360655701</v>
       </c>
       <c r="D3">
-        <v>2.4390243902439001E-2</v>
+        <v>9.7560975609756097E-3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>0.49836065573770499</v>
+        <v>4.59016393442623E-2</v>
       </c>
       <c r="D4">
-        <v>0.22926829268292701</v>
+        <v>2.4390243902439001E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>0.26557377049180297</v>
+        <v>0.49836065573770499</v>
       </c>
       <c r="D5">
-        <v>0.34146341463414598</v>
+        <v>0.22926829268292701</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6">
-        <v>3.27868852459016E-3</v>
+        <v>0.26557377049180297</v>
       </c>
       <c r="D6">
-        <v>1.9512195121951199E-2</v>
+        <v>0.34146341463414598</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7">
-        <v>4.2622950819672101E-2</v>
+        <v>3.27868852459016E-3</v>
       </c>
       <c r="D7">
-        <v>9.2682926829268306E-2</v>
+        <v>1.9512195121951199E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8">
-        <v>0.47213114754098401</v>
+        <v>4.2622950819672101E-2</v>
       </c>
       <c r="D8">
-        <v>0.31219512195122001</v>
+        <v>9.2682926829268306E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>3.9344262295081998E-2</v>
+        <v>0.47213114754098401</v>
       </c>
       <c r="D9">
-        <v>0.10243902439024399</v>
+        <v>0.31219512195122001</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10">
-        <v>0.37049180327868902</v>
+        <v>3.9344262295081998E-2</v>
       </c>
       <c r="D10">
-        <v>0.57073170731707301</v>
+        <v>0.10243902439024399</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11">
-        <v>0.47540983606557402</v>
+        <v>0.37049180327868902</v>
       </c>
       <c r="D11">
-        <v>0.37560975609756098</v>
+        <v>0.57073170731707301</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12">
-        <v>3.2786885245901599E-2</v>
+        <v>0.47540983606557402</v>
       </c>
       <c r="D12">
-        <v>0.12682926829268301</v>
+        <v>0.37560975609756098</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13">
-        <v>4.2622950819672101E-2</v>
+        <v>3.2786885245901599E-2</v>
       </c>
       <c r="D13">
-        <v>7.3170731707317097E-2</v>
+        <v>0.12682926829268301</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14">
-        <v>0.32459016393442602</v>
+        <v>4.2622950819672101E-2</v>
       </c>
       <c r="D14">
-        <v>0.24390243902438999</v>
+        <v>7.3170731707317097E-2</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>0.32459016393442602</v>
+      </c>
+      <c r="D15">
+        <v>0.24390243902438999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>6.5573770491803296E-3</v>
       </c>
-      <c r="D15">
+      <c r="D16">
         <v>4.39024390243902E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>0.14070351758794</v>
+      </c>
+      <c r="D20">
+        <v>6.41025641025641E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>3.5175879396984903E-2</v>
+      </c>
+      <c r="D21">
+        <v>1.9230769230769201E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>0.48241206030150802</v>
+      </c>
+      <c r="D22">
+        <v>0.262820512820513</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23">
+        <v>0.221105527638191</v>
+      </c>
+      <c r="D23">
+        <v>0.32692307692307698</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>5.0251256281407001E-3</v>
+      </c>
+      <c r="D24">
+        <v>2.5641025641025599E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>5.52763819095477E-2</v>
+      </c>
+      <c r="D25">
+        <v>8.3333333333333301E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26">
+        <v>0.42211055276381898</v>
+      </c>
+      <c r="D26">
+        <v>0.30128205128205099</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27">
+        <v>5.0251256281407003E-2</v>
+      </c>
+      <c r="D27">
+        <v>0.108974358974359</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>9</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28">
+        <v>0.34673366834170899</v>
+      </c>
+      <c r="D28">
+        <v>0.56410256410256399</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29">
+        <v>0.42211055276381898</v>
+      </c>
+      <c r="D29">
+        <v>0.35897435897435898</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>11</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30">
+        <v>4.5226130653266298E-2</v>
+      </c>
+      <c r="D30">
+        <v>0.121794871794872</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>12</v>
+      </c>
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31">
+        <v>3.5175879396984903E-2</v>
+      </c>
+      <c r="D31">
+        <v>8.9743589743589702E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>13</v>
+      </c>
+      <c r="B32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32">
+        <v>0.32663316582914598</v>
+      </c>
+      <c r="D32">
+        <v>0.269230769230769</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>14</v>
+      </c>
+      <c r="B33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33">
+        <v>1.00502512562814E-2</v>
+      </c>
+      <c r="D33">
+        <v>4.48717948717949E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <v>0.160377358490566</v>
+      </c>
+      <c r="D37">
+        <v>2.04081632653061E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38">
+        <v>6.6037735849056603E-2</v>
+      </c>
+      <c r="D38">
+        <v>4.08163265306122E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>3</v>
+      </c>
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39">
+        <v>0.52830188679245305</v>
+      </c>
+      <c r="D39">
+        <v>0.122448979591837</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40">
+        <v>0.34905660377358499</v>
+      </c>
+      <c r="D40">
+        <v>0.38775510204081598</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>5</v>
+      </c>
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>6</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42">
+        <v>1.88679245283019E-2</v>
+      </c>
+      <c r="D42">
+        <v>0.122448979591837</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>7</v>
+      </c>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43">
+        <v>0.56603773584905703</v>
+      </c>
+      <c r="D43">
+        <v>0.34693877551020402</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>8</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44">
+        <v>1.88679245283019E-2</v>
+      </c>
+      <c r="D44">
+        <v>8.1632653061224497E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>9</v>
+      </c>
+      <c r="B45" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45">
+        <v>0.41509433962264197</v>
+      </c>
+      <c r="D45">
+        <v>0.59183673469387799</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>10</v>
+      </c>
+      <c r="B46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46">
+        <v>0.57547169811320797</v>
+      </c>
+      <c r="D46">
+        <v>0.42857142857142899</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>11</v>
+      </c>
+      <c r="B47" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47">
+        <v>9.4339622641509396E-3</v>
+      </c>
+      <c r="D47">
+        <v>0.14285714285714299</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>12</v>
+      </c>
+      <c r="B48" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48">
+        <v>5.6603773584905703E-2</v>
+      </c>
+      <c r="D48">
+        <v>2.04081632653061E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>13</v>
+      </c>
+      <c r="B49" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49">
+        <v>0.320754716981132</v>
+      </c>
+      <c r="D49">
+        <v>0.16326530612244899</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>14</v>
+      </c>
+      <c r="B50" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>4.08163265306122E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>